<commit_message>
add new category 'Baby'
</commit_message>
<xml_diff>
--- a/financial_report.xlsx
+++ b/financial_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN4"/>
+  <dimension ref="A1:AP4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,7 +438,7 @@
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="24" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
     <col width="6" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="6" customWidth="1" min="9" max="9"/>
@@ -446,33 +446,35 @@
     <col width="6" customWidth="1" min="11" max="11"/>
     <col width="14" customWidth="1" min="12" max="12"/>
     <col width="6" customWidth="1" min="13" max="13"/>
-    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
     <col width="6" customWidth="1" min="15" max="15"/>
-    <col width="15" customWidth="1" min="16" max="16"/>
+    <col width="8" customWidth="1" min="16" max="16"/>
     <col width="6" customWidth="1" min="17" max="17"/>
-    <col width="10" customWidth="1" min="18" max="18"/>
+    <col width="15" customWidth="1" min="18" max="18"/>
     <col width="6" customWidth="1" min="19" max="19"/>
-    <col width="9" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
     <col width="6" customWidth="1" min="21" max="21"/>
-    <col width="13" customWidth="1" min="22" max="22"/>
+    <col width="9" customWidth="1" min="22" max="22"/>
     <col width="6" customWidth="1" min="23" max="23"/>
-    <col width="10" customWidth="1" min="24" max="24"/>
+    <col width="13" customWidth="1" min="24" max="24"/>
     <col width="6" customWidth="1" min="25" max="25"/>
     <col width="10" customWidth="1" min="26" max="26"/>
     <col width="6" customWidth="1" min="27" max="27"/>
-    <col width="16" customWidth="1" min="28" max="28"/>
+    <col width="9" customWidth="1" min="28" max="28"/>
     <col width="6" customWidth="1" min="29" max="29"/>
-    <col width="10" customWidth="1" min="30" max="30"/>
+    <col width="16" customWidth="1" min="30" max="30"/>
     <col width="6" customWidth="1" min="31" max="31"/>
     <col width="10" customWidth="1" min="32" max="32"/>
     <col width="6" customWidth="1" min="33" max="33"/>
-    <col width="8" customWidth="1" min="34" max="34"/>
+    <col width="10" customWidth="1" min="34" max="34"/>
     <col width="6" customWidth="1" min="35" max="35"/>
-    <col width="9" customWidth="1" min="36" max="36"/>
+    <col width="8" customWidth="1" min="36" max="36"/>
     <col width="6" customWidth="1" min="37" max="37"/>
-    <col width="8" customWidth="1" min="38" max="38"/>
+    <col width="9" customWidth="1" min="38" max="38"/>
     <col width="6" customWidth="1" min="39" max="39"/>
-    <col width="9" customWidth="1" min="40" max="40"/>
+    <col width="8" customWidth="1" min="40" max="40"/>
+    <col width="6" customWidth="1" min="41" max="41"/>
+    <col width="9" customWidth="1" min="42" max="42"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -508,65 +510,70 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
+          <t>Малыш</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>Дом, квартира</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Интернет</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Телефон</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Хоз. Товары</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Продукты</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Отдых</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Спорт/здоровье</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Подписки</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Подарки</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Другое</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Авто</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Отпуск</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Крупняк</t>
         </is>
@@ -579,13 +586,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>118105.32</v>
+        <v>137725.5</v>
       </c>
       <c r="D2" t="n">
-        <v>85699.38</v>
+        <v>46109.09</v>
       </c>
       <c r="F2" t="n">
-        <v>25921.94</v>
+        <v>21263.36</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -633,6 +640,9 @@
         <v>0</v>
       </c>
       <c r="AN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -652,52 +662,55 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>78</v>
+        <v>820</v>
       </c>
       <c r="L3" t="n">
-        <v>1000</v>
+        <v>5678</v>
       </c>
       <c r="N3" t="n">
-        <v>2390</v>
+        <v>1745.18</v>
       </c>
       <c r="P3" t="n">
-        <v>15047.59</v>
+        <v>3785.1</v>
       </c>
       <c r="R3" t="n">
-        <v>86.69</v>
+        <v>5302.15</v>
       </c>
       <c r="T3" t="n">
-        <v>310</v>
+        <v>460</v>
       </c>
       <c r="V3" t="n">
-        <v>13148.66</v>
+        <v>457</v>
       </c>
       <c r="X3" t="n">
-        <v>42676.64</v>
+        <v>6416.26</v>
       </c>
       <c r="Z3" t="n">
-        <v>15477.77</v>
+        <v>25023.52</v>
       </c>
       <c r="AB3" t="n">
-        <v>869</v>
+        <v>14339</v>
       </c>
       <c r="AD3" t="n">
-        <v>398</v>
+        <v>10487</v>
       </c>
       <c r="AF3" t="n">
-        <v>91306.69</v>
+        <v>1138</v>
       </c>
       <c r="AH3" t="n">
-        <v>6363</v>
+        <v>10039.91</v>
       </c>
       <c r="AJ3" t="n">
-        <v>5315.99</v>
+        <v>5159</v>
       </c>
       <c r="AL3" t="n">
-        <v>0</v>
+        <v>3736.05</v>
       </c>
       <c r="AN3" t="n">
-        <v>14000</v>
+        <v>0</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -707,61 +720,64 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>118105.32</v>
+        <v>137725.5</v>
       </c>
       <c r="D4" t="n">
-        <v>85699.38</v>
+        <v>46109.09</v>
       </c>
       <c r="F4" t="n">
-        <v>25921.94</v>
+        <v>21263.36</v>
       </c>
       <c r="J4" t="n">
-        <v>78</v>
+        <v>820</v>
       </c>
       <c r="L4" t="n">
-        <v>1000</v>
+        <v>5678</v>
       </c>
       <c r="N4" t="n">
-        <v>2390</v>
+        <v>1745.18</v>
       </c>
       <c r="P4" t="n">
-        <v>15047.59</v>
+        <v>3785.1</v>
       </c>
       <c r="R4" t="n">
-        <v>86.69</v>
+        <v>5302.15</v>
       </c>
       <c r="T4" t="n">
-        <v>310</v>
+        <v>460</v>
       </c>
       <c r="V4" t="n">
-        <v>13148.66</v>
+        <v>457</v>
       </c>
       <c r="X4" t="n">
-        <v>42676.64</v>
+        <v>6416.26</v>
       </c>
       <c r="Z4" t="n">
-        <v>15477.77</v>
+        <v>25023.52</v>
       </c>
       <c r="AB4" t="n">
-        <v>869</v>
+        <v>14339</v>
       </c>
       <c r="AD4" t="n">
-        <v>398</v>
+        <v>10487</v>
       </c>
       <c r="AF4" t="n">
-        <v>91306.69</v>
+        <v>1138</v>
       </c>
       <c r="AH4" t="n">
-        <v>6363</v>
+        <v>10039.91</v>
       </c>
       <c r="AJ4" t="n">
-        <v>5315.99</v>
+        <v>5159</v>
       </c>
       <c r="AL4" t="n">
-        <v>0</v>
+        <v>3736.05</v>
       </c>
       <c r="AN4" t="n">
-        <v>14000</v>
+        <v>0</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new categoty "Ira"
</commit_message>
<xml_diff>
--- a/financial_report.xlsx
+++ b/financial_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP4"/>
+  <dimension ref="A1:AR4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,31 +450,33 @@
     <col width="6" customWidth="1" min="15" max="15"/>
     <col width="9" customWidth="1" min="16" max="16"/>
     <col width="6" customWidth="1" min="17" max="17"/>
-    <col width="15" customWidth="1" min="18" max="18"/>
+    <col width="9" customWidth="1" min="18" max="18"/>
     <col width="6" customWidth="1" min="19" max="19"/>
-    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="15" customWidth="1" min="20" max="20"/>
     <col width="6" customWidth="1" min="21" max="21"/>
-    <col width="9" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
     <col width="6" customWidth="1" min="23" max="23"/>
-    <col width="13" customWidth="1" min="24" max="24"/>
+    <col width="9" customWidth="1" min="24" max="24"/>
     <col width="6" customWidth="1" min="25" max="25"/>
-    <col width="10" customWidth="1" min="26" max="26"/>
+    <col width="13" customWidth="1" min="26" max="26"/>
     <col width="6" customWidth="1" min="27" max="27"/>
-    <col width="9" customWidth="1" min="28" max="28"/>
+    <col width="10" customWidth="1" min="28" max="28"/>
     <col width="6" customWidth="1" min="29" max="29"/>
-    <col width="16" customWidth="1" min="30" max="30"/>
+    <col width="10" customWidth="1" min="30" max="30"/>
     <col width="6" customWidth="1" min="31" max="31"/>
-    <col width="10" customWidth="1" min="32" max="32"/>
+    <col width="16" customWidth="1" min="32" max="32"/>
     <col width="6" customWidth="1" min="33" max="33"/>
     <col width="10" customWidth="1" min="34" max="34"/>
     <col width="6" customWidth="1" min="35" max="35"/>
-    <col width="10" customWidth="1" min="36" max="36"/>
+    <col width="9" customWidth="1" min="36" max="36"/>
     <col width="6" customWidth="1" min="37" max="37"/>
     <col width="9" customWidth="1" min="38" max="38"/>
     <col width="6" customWidth="1" min="39" max="39"/>
-    <col width="8" customWidth="1" min="40" max="40"/>
+    <col width="9" customWidth="1" min="40" max="40"/>
     <col width="6" customWidth="1" min="41" max="41"/>
-    <col width="9" customWidth="1" min="42" max="42"/>
+    <col width="8" customWidth="1" min="42" max="42"/>
+    <col width="6" customWidth="1" min="43" max="43"/>
+    <col width="12" customWidth="1" min="44" max="44"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -515,65 +517,70 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
+          <t>Ира</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
           <t>Дом, квартира</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Интернет</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Телефон</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Хоз. Товары</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Продукты</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Отдых</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Спорт/здоровье</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Подписки</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Подарки</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Другое</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Авто</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Отпуск</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Крупняк</t>
         </is>
@@ -586,13 +593,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>141074.5</v>
+        <v>231373.65</v>
       </c>
       <c r="D2" t="n">
-        <v>39407.21</v>
+        <v>80126.13</v>
       </c>
       <c r="F2" t="n">
-        <v>55198.21</v>
+        <v>80615.89</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -643,6 +650,9 @@
         <v>0</v>
       </c>
       <c r="AP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -662,55 +672,58 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>394</v>
       </c>
       <c r="L3" t="n">
-        <v>6476</v>
+        <v>10664.79</v>
       </c>
       <c r="N3" t="n">
-        <v>1454</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>6534.62</v>
+        <v>15771.5</v>
       </c>
       <c r="R3" t="n">
-        <v>6119.09</v>
+        <v>11200</v>
       </c>
       <c r="T3" t="n">
+        <v>3996.26</v>
+      </c>
+      <c r="V3" t="n">
         <v>480</v>
       </c>
-      <c r="V3" t="n">
-        <v>440</v>
-      </c>
       <c r="X3" t="n">
-        <v>4598.6</v>
+        <v>640</v>
       </c>
       <c r="Z3" t="n">
-        <v>46721.39</v>
+        <v>4452.81</v>
       </c>
       <c r="AB3" t="n">
-        <v>9280.639999999999</v>
+        <v>32760.53</v>
       </c>
       <c r="AD3" t="n">
-        <v>0</v>
+        <v>20482.56</v>
       </c>
       <c r="AF3" t="n">
-        <v>2438</v>
+        <v>0</v>
       </c>
       <c r="AH3" t="n">
-        <v>10641.97</v>
+        <v>448</v>
       </c>
       <c r="AJ3" t="n">
-        <v>21823.78</v>
+        <v>0</v>
       </c>
       <c r="AL3" t="n">
-        <v>4528.92</v>
+        <v>17251.6</v>
       </c>
       <c r="AN3" t="n">
-        <v>0</v>
+        <v>7112.43</v>
       </c>
       <c r="AP3" t="n">
-        <v>38500</v>
+        <v>0</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>1177357.91</v>
       </c>
     </row>
     <row r="4">
@@ -720,64 +733,67 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>141074.5</v>
+        <v>231373.65</v>
       </c>
       <c r="D4" t="n">
-        <v>39407.21</v>
+        <v>80126.13</v>
       </c>
       <c r="F4" t="n">
-        <v>55198.21</v>
+        <v>80615.89</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>394</v>
       </c>
       <c r="L4" t="n">
-        <v>6476</v>
+        <v>10664.79</v>
       </c>
       <c r="N4" t="n">
-        <v>1454</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>6534.62</v>
+        <v>15771.5</v>
       </c>
       <c r="R4" t="n">
-        <v>6119.09</v>
+        <v>11200</v>
       </c>
       <c r="T4" t="n">
+        <v>3996.26</v>
+      </c>
+      <c r="V4" t="n">
         <v>480</v>
       </c>
-      <c r="V4" t="n">
-        <v>440</v>
-      </c>
       <c r="X4" t="n">
-        <v>4598.6</v>
+        <v>640</v>
       </c>
       <c r="Z4" t="n">
-        <v>46721.39</v>
+        <v>4452.81</v>
       </c>
       <c r="AB4" t="n">
-        <v>9280.639999999999</v>
+        <v>32760.53</v>
       </c>
       <c r="AD4" t="n">
-        <v>0</v>
+        <v>20482.56</v>
       </c>
       <c r="AF4" t="n">
-        <v>2438</v>
+        <v>0</v>
       </c>
       <c r="AH4" t="n">
-        <v>10641.97</v>
+        <v>448</v>
       </c>
       <c r="AJ4" t="n">
-        <v>21823.78</v>
+        <v>0</v>
       </c>
       <c r="AL4" t="n">
-        <v>4528.92</v>
+        <v>17251.6</v>
       </c>
       <c r="AN4" t="n">
-        <v>0</v>
+        <v>7112.43</v>
       </c>
       <c r="AP4" t="n">
-        <v>38500</v>
+        <v>0</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>1177357.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add fifancial_report to gitignore
</commit_message>
<xml_diff>
--- a/financial_report.xlsx
+++ b/financial_report.xlsx
@@ -434,21 +434,21 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="9" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="24" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
-    <col width="9" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
     <col width="6" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="6" customWidth="1" min="9" max="9"/>
     <col width="8" customWidth="1" min="10" max="10"/>
     <col width="6" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="14" customWidth="1" min="12" max="12"/>
     <col width="6" customWidth="1" min="13" max="13"/>
     <col width="10" customWidth="1" min="14" max="14"/>
     <col width="6" customWidth="1" min="15" max="15"/>
-    <col width="8" customWidth="1" min="16" max="16"/>
+    <col width="9" customWidth="1" min="16" max="16"/>
     <col width="6" customWidth="1" min="17" max="17"/>
     <col width="9" customWidth="1" min="18" max="18"/>
     <col width="6" customWidth="1" min="19" max="19"/>
@@ -462,15 +462,15 @@
     <col width="6" customWidth="1" min="27" max="27"/>
     <col width="10" customWidth="1" min="28" max="28"/>
     <col width="6" customWidth="1" min="29" max="29"/>
-    <col width="10" customWidth="1" min="30" max="30"/>
+    <col width="20" customWidth="1" min="30" max="30"/>
     <col width="6" customWidth="1" min="31" max="31"/>
     <col width="16" customWidth="1" min="32" max="32"/>
     <col width="6" customWidth="1" min="33" max="33"/>
     <col width="10" customWidth="1" min="34" max="34"/>
     <col width="6" customWidth="1" min="35" max="35"/>
-    <col width="9" customWidth="1" min="36" max="36"/>
+    <col width="10" customWidth="1" min="36" max="36"/>
     <col width="6" customWidth="1" min="37" max="37"/>
-    <col width="20" customWidth="1" min="38" max="38"/>
+    <col width="9" customWidth="1" min="38" max="38"/>
     <col width="6" customWidth="1" min="39" max="39"/>
     <col width="9" customWidth="1" min="40" max="40"/>
     <col width="6" customWidth="1" min="41" max="41"/>
@@ -593,13 +593,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>128791.79</v>
+        <v>196698.69</v>
       </c>
       <c r="D2" t="n">
-        <v>43599.25</v>
+        <v>33934.72</v>
       </c>
       <c r="F2" t="n">
-        <v>20052</v>
+        <v>43400.11</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -672,58 +672,58 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="L3" t="n">
-        <v>4221.940000000001</v>
+        <v>3374.96</v>
       </c>
       <c r="N3" t="n">
-        <v>7678</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>7547.2</v>
+        <v>18448.4</v>
       </c>
       <c r="R3" t="n">
-        <v>10000</v>
+        <v>11509.5</v>
       </c>
       <c r="T3" t="n">
-        <v>40209.9</v>
+        <v>40217.86</v>
       </c>
       <c r="V3" t="n">
         <v>480</v>
       </c>
       <c r="X3" t="n">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="Z3" t="n">
-        <v>8912.58</v>
+        <v>11700.11</v>
       </c>
       <c r="AB3" t="n">
-        <v>39616.52</v>
+        <v>37776.71</v>
       </c>
       <c r="AD3" t="n">
-        <v>12496.86</v>
+        <v>3787.07</v>
       </c>
       <c r="AF3" t="n">
-        <v>0</v>
+        <v>9770</v>
       </c>
       <c r="AH3" t="n">
-        <v>4943.05</v>
+        <v>3541.98</v>
       </c>
       <c r="AJ3" t="n">
-        <v>31800</v>
+        <v>10664.91</v>
       </c>
       <c r="AL3" t="n">
-        <v>10571.88</v>
+        <v>16455</v>
       </c>
       <c r="AN3" t="n">
-        <v>5995.18</v>
+        <v>6959.09</v>
       </c>
       <c r="AP3" t="n">
         <v>0</v>
       </c>
       <c r="AR3" t="n">
-        <v>950462</v>
+        <v>122658</v>
       </c>
     </row>
     <row r="4">
@@ -733,67 +733,67 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>128791.79</v>
+        <v>196698.69</v>
       </c>
       <c r="D4" t="n">
-        <v>43599.25</v>
+        <v>33934.72</v>
       </c>
       <c r="F4" t="n">
-        <v>20052</v>
+        <v>43400.11</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="L4" t="n">
-        <v>4221.940000000001</v>
+        <v>3374.96</v>
       </c>
       <c r="N4" t="n">
-        <v>7678</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>7547.2</v>
+        <v>18448.4</v>
       </c>
       <c r="R4" t="n">
-        <v>10000</v>
+        <v>11509.5</v>
       </c>
       <c r="T4" t="n">
-        <v>40209.9</v>
+        <v>40217.86</v>
       </c>
       <c r="V4" t="n">
         <v>480</v>
       </c>
       <c r="X4" t="n">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="Z4" t="n">
-        <v>8912.58</v>
+        <v>11700.11</v>
       </c>
       <c r="AB4" t="n">
-        <v>39616.52</v>
+        <v>37776.71</v>
       </c>
       <c r="AD4" t="n">
-        <v>12496.86</v>
+        <v>3787.07</v>
       </c>
       <c r="AF4" t="n">
-        <v>0</v>
+        <v>9770</v>
       </c>
       <c r="AH4" t="n">
-        <v>4943.05</v>
+        <v>3541.98</v>
       </c>
       <c r="AJ4" t="n">
-        <v>31800</v>
+        <v>10664.91</v>
       </c>
       <c r="AL4" t="n">
-        <v>10571.88</v>
+        <v>16455</v>
       </c>
       <c r="AN4" t="n">
-        <v>5995.18</v>
+        <v>6959.09</v>
       </c>
       <c r="AP4" t="n">
         <v>0</v>
       </c>
       <c r="AR4" t="n">
-        <v>950462</v>
+        <v>122658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>